<commit_message>
remove column 7 & modify path in Prediction.py
</commit_message>
<xml_diff>
--- a/data/classification.xlsx
+++ b/data/classification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Grad_School_Year_1\Fire Safety Project - NRC\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/kentwhf_wu_mail_utoronto_ca/Documents/NSERC MIE 2021/Fire_Safety/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFAC723-E446-40C9-9AD4-07EFC69F5AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CCFAC723-E446-40C9-9AD4-07EFC69F5AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69EA39CA-A3EF-4D64-A4F1-E096D864A528}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="86">
   <si>
     <t>CO2</t>
   </si>
@@ -148,12 +148,6 @@
   </si>
   <si>
     <t>oxidizing</t>
-  </si>
-  <si>
-    <t>oxidizing flame</t>
-  </si>
-  <si>
-    <t>phosgen</t>
   </si>
   <si>
     <t>methylmethacrylate</t>
@@ -922,7 +916,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ABC966B5-E680-4491-9266-DC0343994775}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ABC966B5-E680-4491-9266-DC0343994775}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="7">
     <pivotField showAll="0">
@@ -1220,25 +1214,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>30</v>
       </c>
@@ -1249,16 +1243,16 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,7 +1275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1304,7 +1298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1327,7 +1321,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1344,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1396,7 +1390,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1419,7 +1413,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1427,7 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
         <v>32</v>
@@ -1442,7 +1436,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1456,7 +1450,7 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
         <v>32</v>
@@ -1465,7 +1459,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1473,7 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
@@ -1488,7 +1482,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1511,7 +1505,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1528,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1556,11 +1550,8 @@
       <c r="G14" t="s">
         <v>32</v>
       </c>
-      <c r="H14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1582,11 +1573,8 @@
       <c r="G15" t="s">
         <v>32</v>
       </c>
-      <c r="H15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1588,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
         <v>33</v>
@@ -1609,7 +1597,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1623,7 +1611,7 @@
         <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
         <v>32</v>
@@ -1632,7 +1620,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1655,7 +1643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1669,7 +1657,7 @@
         <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
         <v>32</v>
@@ -1678,7 +1666,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1701,7 +1689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1724,7 +1712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1747,7 +1735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1758,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1793,7 +1781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1816,7 +1804,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1830,7 +1818,7 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
         <v>32</v>
@@ -1839,7 +1827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -1853,7 +1841,7 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
         <v>32</v>
@@ -1862,7 +1850,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -1876,7 +1864,7 @@
         <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F28" t="s">
         <v>33</v>
@@ -1885,7 +1873,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
@@ -1907,11 +1895,8 @@
       <c r="G29" t="s">
         <v>33</v>
       </c>
-      <c r="H29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -1934,7 +1919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
@@ -1957,9 +1942,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
@@ -1994,97 +1979,97 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="22"/>
       <c r="C4" s="23"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="22"/>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="23"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="23"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="22"/>
       <c r="C17" s="23"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="22"/>
       <c r="C18" s="23"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -2098,105 +2083,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2211,7 +2196,7 @@
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -2220,9 +2205,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" t="s">
@@ -2244,87 +2229,87 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" t="s">
@@ -2346,9 +2331,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" t="s">
@@ -2370,9 +2355,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" t="s">
@@ -2394,9 +2379,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" t="s">
@@ -2418,9 +2403,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" t="s">
@@ -2442,7 +2427,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
@@ -2466,9 +2451,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" t="s">
@@ -2490,9 +2475,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" t="s">
@@ -2514,12 +2499,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -2540,9 +2525,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" t="s">
@@ -2564,9 +2549,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -2587,9 +2572,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -2613,222 +2598,222 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="C30" t="s">
         <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>33</v>
@@ -2843,9 +2828,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
@@ -2880,15 +2865,15 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>9.5/100</f>
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1*1000000</f>
         <v>95000</v>

</xml_diff>